<commit_message>
Modificações de pastas de configurações
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,10 @@
     <font>
       <name val="Arial"/>
       <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -51,9 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -421,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +452,30 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>https://spelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>contato@spelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadoreskorman.com.br/empresas-elevadores-sao-paulo</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>korman@elevadoreskorman.com.br;comercial@elevadoreskorman.com.br;vendas@elevadoreskorman.com.br;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajuste ao iniciar robo
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,10 +28,6 @@
     <font>
       <name val="Arial"/>
       <b val="1"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -55,12 +51,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -428,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,90 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>https://spelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>contato@spelevadores.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>https://www.elevadoreskorman.com.br/empresas-elevadores-sao-paulo</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>korman@elevadoreskorman.com.br;comercial@elevadoreskorman.com.br;vendas@elevadoreskorman.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>http://www.emelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>contato@emelevadores.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>https://coteibem.sindiconet.com.br/fornecedores/manutencao-elevadores/sp/sao-paulo</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>contato@coteibem.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>https://continentalelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>continentalelevadores@protonmail.com;</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>http://primac.com.br/</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>comercial@primac.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>https://retrofitelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>contato@elevadoresretrofit.com.br;</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Inclusão de Busca pelo Google com mecanismo anti-decção de bot
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,72 +455,24 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>https://spelevadores.com.br/</t>
+          <t>https://iesab.com.br/preco-do-elevador-residencial/#:~:text=M%C3%A9dia%20de%20pre%C3%A7o%20do%20Elevador,comprimento%2C%20menor%20ser%C3%A1%20o%20custo.</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>contato@spelevadores.com.br;</t>
+          <t>emailbit21@gmail.com;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>https://www.elevadoreskorman.com.br/empresas-elevadores-sao-paulo</t>
+          <t>https://coteibem.sindiconet.com.br/fornecedores/manutencao-elevadores/sp/sao-paulo</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>vendas@elevadoreskorman.com.br;korman@elevadoreskorman.com.br;comercial@elevadoreskorman.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>http://www.emelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>contato@emelevadores.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>https://coteibem.sindiconet.com.br/fornecedores/manutencao-elevadores/sp/sao-paulo</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
           <t>contato@coteibem.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>http://primac.com.br/</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>comercial@primac.com.br;</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>https://retrofitelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>contato@elevadoresretrofit.com.br;</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusão de opções de browsers
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,12 +455,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>https://iesab.com.br/preco-do-elevador-residencial/#:~:text=M%C3%A9dia%20de%20pre%C3%A7o%20do%20Elevador,comprimento%2C%20menor%20ser%C3%A1%20o%20custo.</t>
+          <t>https://villarta.com.br/elevadores-e-escadas-rolantes-villarta/lista-de-empresas-de-elevadores-em-sp/</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>emailbit21@gmail.com;</t>
+          <t>protecaodedados@villarta.com.br;</t>
         </is>
       </c>
     </row>
@@ -473,6 +473,78 @@
       <c r="B3" s="2" t="inlineStr">
         <is>
           <t>contato@coteibem.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>https://spelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>contato@spelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>https://www.basselevadores.com.br/elevadores-sao-paulo-sp.php</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>contato@basselevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>https://elevadoresoiwa.com.br/</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>comercial@elevadoresoiwa.com.br;oiwa@elevadoresoiwa.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>https://www.otis.com/pt/br</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Navigati_ouvidoria@otis.com;ouvidoria@otis.com;Navigati_imprensa@otis.com;cac@otis.com;imprensa@otis.com;</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>https://crel.com.br/</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>bruno@crel.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>https://www.primac.com.br/manutencao-de-elevadores-sp.php</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>comercial@primac.com.br;</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajustes no robo para encerramento
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,60 +455,612 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>https://coteibem.sindiconet.com.br/fornecedores/manutencao-elevadores/sp/sao-paulo</t>
+          <t>https://iesab.com.br/preco-do-elevador-residencial/#:~:text=M%C3%A9dia%20de%20pre%C3%A7o%20do%20Elevador,comprimento%2C%20menor%20ser%C3%A1%20o%20custo.</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>contato@coteibem.com.br;</t>
+          <t>emailbit21@gmail.com;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>https://spelevadores.com.br/</t>
+          <t>https://condolivre.com.br/gestao-financeira/quanto-cobrar-por-manutencao-de-elevadores/#:~:text=A%20manuten%C3%A7%C3%A3o%20preventiva%20de%20elevadores,e%20da%20complexidade%20do%20equipamento.</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>contato@spelevadores.com.br;</t>
+          <t>contato@condolivre.com.br;flags@2x.png;</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>https://villarta.com.br/elevadores-e-escadas-rolantes-villarta/lista-de-empresas-de-elevadores-em-sp/</t>
+          <t>https://coteibem.sindiconet.com.br/fornecedores/manutencao-elevadores/sp/sao-paulo</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>protecaodedados@villarta.com.br;</t>
+          <t>contato@coteibem.com.br;</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>https://crel.com.br/</t>
+          <t>https://spelevadores.com.br/</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>bruno@crel.com.br;</t>
+          <t>contato@spelevadores.com.br;</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
+          <t>https://villarta.com.br/elevadores-e-escadas-rolantes-villarta/lista-de-empresas-de-elevadores-em-sp/</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>protecaodedados@villarta.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>https://www.basselevadores.com.br/elevadores-sao-paulo-sp.php</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>contato@basselevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
           <t>https://elevadoresoiwa.com.br/</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>oiwa@elevadoresoiwa.com.br;comercial@elevadoresoiwa.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>https://www.otis.com/pt/br</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>cac@otis.com;navigati_cac@otis.com;imprensa@otis.com;navigati_imprensa@otis.com;ouvidoria@otis.com;</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>https://www.primac.com.br/manutencao-de-elevadores-sp.php</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>comercial@primac.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>https://www.rayteckelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>rayteck@rayteckelevadores.com.br;605a7baede844d278b89dc95ae0a9123@sentry-next.wixpress.com;8c4075d5481d476e945486754f783364@sentry.io;dd0a55ccb8124b9c9d938e3acf41f8aa@sentry.wixpress.com;c183baa23371454f99f417f6616b724d@sentry.wixpress.com;</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>https://nextelevadores.com/</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>hudsonkanegae@gatecubetecnologia.com;</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>https://www.monciel.com.br/empresa-de-elevadores.php</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>monciel@monciel.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>https://crel.com.br/</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>bruno@crel.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>https://www.designelevadores.com.br/empresa-de-elevadores-em-sao-paulo.php</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>contato@designelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>https://www.econodata.com.br/maiores-empresas/sp-sao-paulo/busca-elevadores</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>20348-featured-260x140@1.5x.jpg;20348-featured-260x140@2x.jpg;20348-featured-260x140@2.5x.jpg;20348-featured-260x140@3x.jpg;20391-featured-260x140@1.5x.jpg;</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadoreskorman.com.br/empresas-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>korman@elevadoreskorman.com.br;vendas@elevadoreskorman.com.br;comercial@elevadoreskorman.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>https://europaelevadores.com.br/manutencao-de-elevadores-em-sp/</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>europa@europaelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>https://www.surmonter.com.br/empresa-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>vendas@surmonter.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>https://www.hts.com.br/</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>contato@hts.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>https://www.ultronelevadores.com.br/empresas-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>contato@ultronelevadores.com.br;naoinformado@naoinformado.com;</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>https://www.framartelelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>framartelelevadores@terra.com.br;elcio_30@hotmail.com;</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>https://www.mmelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>orcamentos2@g7elevadores.com.br;comercial2@mmelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>https://www.gmvelevadores.com.br/hs/elevadores-em-sao-paulo/</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>cropped-favicon@2x-pichi-32x32.png;cropped-favicon@2x-pichi-192x192.png;cropped-favicon@2x-pichi-180x180.png;cropped-favicon@2x-pichi-270x270.png;contato@gmvelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>https://www.hardee.com.br/empresas-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>hardee@hardee.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>https://www.tecnewelevadores.com.br/manutencao-de-elevadores-em-sao-paulo</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>tecnica@tecnewelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>https://www.arsenalelevadores.com.br/empresas-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>arsenal@arsenalelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>https://espel.com.br/</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>espel@espel.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>https://atselevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>contato@atselevadores.com.br;info@atselevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>https://www.flexst.com.br/empresa-elevadores-escadas-rolantes-sp</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>vendas@flexelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>https://novitaelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>contato@novitaelevadores.com.br;novita@novitaelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>https://retrofitelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>contato@elevadoresretrofit.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>https://rcelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>rcelevadores@hotmail.com;</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>http://orionlift.com.br/</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>faleconosco@orionlift.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadorestakaoki.com.br/</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>atendimento@elevadorestakaoki.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>https://elevatis.com.br/</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>rogerio.teodoro@elevatis.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>https://www.astroselevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>contato@astroselevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>https://sselev.com.br/</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>contato@sselev.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>https://basicelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>basic@basicelevadores.com.br;litoral@basicelevadores.com.br;campinas@basicelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadoresfavaretto.com.br/</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>contato@elevadoresfavaretto.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>https://www.polielevadores.com.br/venda-de-elevadores-em-sp.php</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>contato@polielevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>https://elevapro.com.br/</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>20riziarowe@gmail.com;20comercial@elevapro.com.br;comercial@elevapro.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadoreshertz.com.br/empresa-desmontagem-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="inlineStr">
+        <is>
+          <t>comercial@elevadoreshertz.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>https://www.estiloelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>operacional@estiloelevadores.com.br;engenharia@estiloelevadores.com.br;andrejan.silva@estiloelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>https://elevac.com.br/</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
+        <is>
+          <t>vendas@elevac.com.br;vendas1@elevac.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>https://rvmanutencao.com.br/</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>atendimento@rvmanutencao.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>https://www.mblelevadores.com.br/manutencao-de-elevadores-em-sp.php</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>vendas@mblelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadoresupline.com.br/manutencao-elevadores-empresas</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>atendimento@elevadoresupline.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>https://seciesp.com.br/</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr">
+        <is>
+          <t>seciesp@seciesp.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>https://askelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>atendimento@askelevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>https://acselevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr">
+        <is>
+          <t>comercial@acselevadores.com.br;</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>http://eleribelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>contato@eleribelevadores.com.br;</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mudança no mecanismo de validação de e-mail
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,415 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>emailbit21@gmail.com;</t>
+          <t>emailbit21@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>https://condolivre.com.br/gestao-financeira/quanto-cobrar-por-manutencao-de-elevadores/#:~:text=A%20manuten%C3%A7%C3%A3o%20preventiva%20de%20elevadores,e%20da%20complexidade%20do%20equipamento.</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>contato@condolivre.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>https://coteibem.sindiconet.com.br/fornecedores/manutencao-elevadores/sp/sao-paulo</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>contato@coteibem.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>https://spelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>contato@spelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>https://villarta.com.br/elevadores-e-escadas-rolantes-villarta/lista-de-empresas-de-elevadores-em-sp/</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>protecaodedados@villarta.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>https://www.basselevadores.com.br/elevadores-sao-paulo-sp.php</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>contato@basselevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>https://elevadoresoiwa.com.br/</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>oiwa@elevadoresoiwa.com.br;comercial@elevadoresoiwa.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>https://www.otis.com/pt/br</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>cac@otis.com;navigati_cac@otis.com;imprensa@otis.com;navigati_imprensa@otis.com;ouvidoria@otis.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>https://www.primac.com.br/manutencao-de-elevadores-sp.php</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>comercial@primac.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>https://www.rayteckelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>rayteck@rayteckelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>https://nextelevadores.com/</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>hudsonkanegae@gatecubetecnologia.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>https://www.monciel.com.br/empresa-de-elevadores.php</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>monciel@monciel.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>https://crel.com.br/</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>bruno@crel.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>https://www.designelevadores.com.br/empresa-de-elevadores-em-sao-paulo.php</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>contato@designelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadoreskorman.com.br/empresas-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>korman@elevadoreskorman.com.br;vendas@elevadoreskorman.com.br;comercial@elevadoreskorman.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>https://europaelevadores.com.br/manutencao-de-elevadores-em-sp/</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>europa@europaelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>https://www.surmonter.com.br/empresa-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>vendas@surmonter.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>https://www.ultronelevadores.com.br/empresas-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>contato@ultronelevadores.com.br;naoinformado@naoinformado.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>https://www.hts.com.br/</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>contato@hts.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>https://www.framartelelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>framartelelevadores@terra.com.br;elcio_30@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>https://www.mmelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>orcamentos2@g7elevadores.com.br;comercial2@mmelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>https://www.gmvelevadores.com.br/hs/elevadores-em-sao-paulo/</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>contato@gmvelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>https://www.tecnewelevadores.com.br/manutencao-de-elevadores-em-sao-paulo</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>tecnica@tecnewelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>https://www.arsenalelevadores.com.br/empresas-elevadores-sp</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>arsenal@arsenalelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>https://espel.com.br/</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>espel@espel.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>https://atselevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>contato@atselevadores.com.br;info@atselevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>https://www.flexst.com.br/empresa-elevadores-escadas-rolantes-sp</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>vendas@flexelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>https://novitaelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>contato@novitaelevadores.com.br;novita@novitaelevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>https://rcelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>rcelevadores@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>http://orionlift.com.br/</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>faleconosco@orionlift.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>https://elevatis.com.br/</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>rogerio.teodoro@elevatis.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>https://retrofitelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>contato@elevadoresretrofit.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>https://www.astroselevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>contato@astroselevadores.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>https://sselev.com.br/</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>contato@sselev.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadorestakaoki.com.br/</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>atendimento@elevadorestakaoki.com.br</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mudança no mecanismo de validação de telefone
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,7 @@
   <cols>
     <col width="50" customWidth="1" min="1" max="1"/>
     <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -451,6 +452,11 @@
           <t>email</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>telefone</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -463,6 +469,11 @@
           <t>emailbit21@gmail.com</t>
         </is>
       </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>(31) 3212-1604;</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -475,400 +486,60 @@
           <t>contato@condolivre.com.br</t>
         </is>
       </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>(11) 3097-9918;(11) 94223-2039;(11) 98084-1487;</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>https://coteibem.sindiconet.com.br/fornecedores/manutencao-elevadores/sp/sao-paulo</t>
+          <t>https://spelevadores.com.br/</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>contato@coteibem.com.br</t>
+          <t>contato@spelevadores.com.br</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>(11) 2353-5320;</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>https://spelevadores.com.br/</t>
+          <t>https://villarta.com.br/elevadores-e-escadas-rolantes-villarta/lista-de-empresas-de-elevadores-em-sp/</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>contato@spelevadores.com.br</t>
+          <t>protecaodedados@villarta.com.br</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>(11) 3346-8811;(11) 91364-5830;</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>https://villarta.com.br/elevadores-e-escadas-rolantes-villarta/lista-de-empresas-de-elevadores-em-sp/</t>
+          <t>https://www.basselevadores.com.br/elevadores-sao-paulo-sp.php</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>protecaodedados@villarta.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>https://www.basselevadores.com.br/elevadores-sao-paulo-sp.php</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
           <t>contato@basselevadores.com.br</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>https://elevadoresoiwa.com.br/</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>oiwa@elevadoresoiwa.com.br;comercial@elevadoresoiwa.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>https://www.otis.com/pt/br</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>cac@otis.com;navigati_cac@otis.com;imprensa@otis.com;navigati_imprensa@otis.com;ouvidoria@otis.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>https://www.primac.com.br/manutencao-de-elevadores-sp.php</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>comercial@primac.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>https://www.rayteckelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>rayteck@rayteckelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>https://nextelevadores.com/</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>hudsonkanegae@gatecubetecnologia.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>https://www.monciel.com.br/empresa-de-elevadores.php</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>monciel@monciel.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>https://crel.com.br/</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>bruno@crel.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>https://www.designelevadores.com.br/empresa-de-elevadores-em-sao-paulo.php</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>contato@designelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>https://www.elevadoreskorman.com.br/empresas-elevadores-sp</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>korman@elevadoreskorman.com.br;vendas@elevadoreskorman.com.br;comercial@elevadoreskorman.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>https://europaelevadores.com.br/manutencao-de-elevadores-em-sp/</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>europa@europaelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>https://www.surmonter.com.br/empresa-elevadores-sp</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>vendas@surmonter.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>https://www.ultronelevadores.com.br/empresas-elevadores-sp</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>contato@ultronelevadores.com.br;naoinformado@naoinformado.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>https://www.hts.com.br/</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>contato@hts.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>https://www.framartelelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>framartelelevadores@terra.com.br;elcio_30@hotmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>https://www.mmelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>orcamentos2@g7elevadores.com.br;comercial2@mmelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>https://www.gmvelevadores.com.br/hs/elevadores-em-sao-paulo/</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="inlineStr">
-        <is>
-          <t>contato@gmvelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>https://www.tecnewelevadores.com.br/manutencao-de-elevadores-em-sao-paulo</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>tecnica@tecnewelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>https://www.arsenalelevadores.com.br/empresas-elevadores-sp</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>arsenal@arsenalelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>https://espel.com.br/</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>espel@espel.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>https://atselevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>contato@atselevadores.com.br;info@atselevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>https://www.flexst.com.br/empresa-elevadores-escadas-rolantes-sp</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>vendas@flexelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>https://novitaelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>contato@novitaelevadores.com.br;novita@novitaelevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>https://rcelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>rcelevadores@hotmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>http://orionlift.com.br/</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>faleconosco@orionlift.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>https://elevatis.com.br/</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t>rogerio.teodoro@elevatis.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>https://retrofitelevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>contato@elevadoresretrofit.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>https://www.astroselevadores.com.br/</t>
-        </is>
-      </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>contato@astroselevadores.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>https://sselev.com.br/</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>contato@sselev.com.br</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="inlineStr">
-        <is>
-          <t>https://www.elevadorestakaoki.com.br/</t>
-        </is>
-      </c>
-      <c r="B36" s="2" t="inlineStr">
-        <is>
-          <t>atendimento@elevadorestakaoki.com.br</t>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>(11) 3934-4855;</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refatoração completa antes de inicio dos testes unitários
</commit_message>
<xml_diff>
--- a/output/empresas.xlsx
+++ b/output/empresas.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,10 @@
     <font>
       <name val="Arial"/>
       <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -51,9 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -421,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +458,125 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>http://www.emelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>contato@emelevadores.com.br;</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>(11) 2035-1975;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>https://www.elevadoreskorman.com.br/empresas-elevadores-sao-paulo</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>korman@elevadoreskorman.com.br;comercial@elevadoreskorman.com.br;vendas@elevadoreskorman.com.br;</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>(11) 2914-0248;(11) 2914-7506;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>https://retrofitelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>contato@elevadoresretrofit.com.br;</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>(11) 98942-8956;</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>http://primac.com.br/</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>comercial@primac.com.br;</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>(11) 2942-7479;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>https://iesab.com.br/preco-do-elevador-residencial/#:~:text=M%C3%A9dia%20de%20pre%C3%A7o%20do%20Elevador,comprimento%2C%20menor%20ser%C3%A1%20o%20custo.</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>emailbit21@gmail.com;</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>(31) 3212-1604;</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>https://spelevadores.com.br/</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>contato@spelevadores.com.br;</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>(11) 2353-5320;</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>https://villarta.com.br/elevadores-e-escadas-rolantes-villarta/lista-de-empresas-de-elevadores-em-sp/</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>protecaodedados@villarta.com.br;</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>(11) 91364-5830;(11) 3346-8811;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>